<commit_message>
maricopa long results update
</commit_message>
<xml_diff>
--- a/Simple RNN results May to Aug/May to Aug Prediction.xlsx
+++ b/Simple RNN results May to Aug/May to Aug Prediction.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alano\evaptransmission\Simple RNN results May to Aug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FDDF97-46A1-451C-AB3A-915CEDE2DF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB33D54-000D-4E5D-AADD-CEA8D7BAD511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3135" windowWidth="21600" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17685" yWindow="6060" windowWidth="21600" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Maricopa" sheetId="5" r:id="rId1"/>
+    <sheet name="Maricopa" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -336,11 +336,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBA3366-F5C5-41BD-90EE-930DBC8EEB32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A96"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>